<commit_message>
add utf-8 support and fix ided2_videojuegos error
</commit_message>
<xml_diff>
--- a/ided2_videojuegos.xlsx
+++ b/ided2_videojuegos.xlsx
@@ -317,8 +317,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1169,12 +1169,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="n">
-        <f aca="false">SUM(B2:B60)</f>
-        <v>138</v>
-      </c>
-    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1198,11 +1193,11 @@
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>